<commit_message>
"Subo el tablero de control de calidad"
</commit_message>
<xml_diff>
--- a/Proyectos_Detalles.xlsx
+++ b/Proyectos_Detalles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Personal\Desktop\Power Bi - Proyectos\Portfolio_Streamlit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B714A7DB-3ACE-4255-8257-0B26C1ECB311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313E1388-9BD0-426D-A607-26256BBECD5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12456" xr2:uid="{244D0D7B-CEB5-420A-B1AE-6D23D79DB64F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{244D0D7B-CEB5-420A-B1AE-6D23D79DB64F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>https://app.powerbi.com/view?r=eyJrIjoiNDA5NmQzY2UtYTY3ZS00ZDFmLWJkOTYtMTMyOTM5MGYyOTlmIiwidCI6IjkxZjVjYjg5LTUyZmUtNDdhYi05MDVmLTRlMzU4ODZmNWE1NyIsImMiOjR9</t>
   </si>
@@ -103,6 +103,18 @@
   </si>
   <si>
     <t>Descripcion</t>
+  </si>
+  <si>
+    <t>https://app.powerbi.com/view?r=eyJrIjoiYTFjNTgxMjUtOWJlZS00ODJjLTlhYmItOGEyOWRjOTdmZGZhIiwidCI6IjkxZjVjYjg5LTUyZmUtNDdhYi05MDVmLTRlMzU4ODZmNWE1NyIsImMiOjR9</t>
+  </si>
+  <si>
+    <t>portada_proyecto_005.png</t>
+  </si>
+  <si>
+    <t>Control de calidad</t>
+  </si>
+  <si>
+    <t>Proy_TCon_003</t>
   </si>
 </sst>
 </file>
@@ -134,7 +146,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -157,21 +169,189 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -182,6 +362,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{77884F4D-EAF6-4CE6-A7F9-80362DD9B3E4}" name="Tabla1" displayName="Tabla1" ref="A1:E6" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="7">
+  <autoFilter ref="A1:E6" xr:uid="{77884F4D-EAF6-4CE6-A7F9-80362DD9B3E4}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{FF02AA83-C173-4DC0-9A0D-43ECBFC0CB7A}" name="Referencia" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{14269345-09BB-4003-8577-05A9C36CF3E7}" name="Nombre" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{0BB2FA58-F730-4AC5-AA32-15EFFC57F47F}" name="Img" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{E2A7E7A3-8DCC-418E-A469-34D77540A871}" name="link" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{43FF2470-7820-4867-8A73-7578B15185D5}" name="Descripcion" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -481,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3001F80C-2A16-4247-B431-82C5DCED0A36}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,24 +691,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -531,7 +725,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -548,7 +742,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -565,7 +759,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -579,6 +773,20 @@
       </c>
       <c r="E5" s="1" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -587,5 +795,8 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Proyecto Ordenes de compra
</commit_message>
<xml_diff>
--- a/Proyectos_Detalles.xlsx
+++ b/Proyectos_Detalles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Personal\Desktop\Power Bi - Proyectos\Portfolio_Streamlit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED60EE9-CFF3-4FC7-A18D-1D95035F3DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CFC0A16-2CAD-44B2-85E5-C7C28A4CCD0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="14064" windowWidth="21600" windowHeight="11232" xr2:uid="{244D0D7B-CEB5-420A-B1AE-6D23D79DB64F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{244D0D7B-CEB5-420A-B1AE-6D23D79DB64F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>https://app.powerbi.com/view?r=eyJrIjoiNDA5NmQzY2UtYTY3ZS00ZDFmLWJkOTYtMTMyOTM5MGYyOTlmIiwidCI6IjkxZjVjYjg5LTUyZmUtNDdhYi05MDVmLTRlMzU4ODZmNWE1NyIsImMiOjR9</t>
   </si>
@@ -163,6 +163,18 @@
   </si>
   <si>
     <t>https://app.powerbi.com/view?r=eyJrIjoiMDUxNDBlYzctNjhmMC00ZjMxLWExMWItNzYyNzNiNDlkZmU2IiwidCI6IjkxZjVjYjg5LTUyZmUtNDdhYi05MDVmLTRlMzU4ODZmNWE1NyIsImMiOjR9</t>
+  </si>
+  <si>
+    <t>Seguimiento de Ocs</t>
+  </si>
+  <si>
+    <t>Proy_TCon_005</t>
+  </si>
+  <si>
+    <t>portada_proyecto_010.png</t>
+  </si>
+  <si>
+    <t>https://app.powerbi.com/view?r=eyJrIjoiYzUyMDdmNmUtY2Y1Yy00YzY2LWJmZDQtZGIyMTQyYjQ1OTJmIiwidCI6IjkxZjVjYjg5LTUyZmUtNDdhYi05MDVmLTRlMzU4ODZmNWE1NyIsImMiOjR9</t>
   </si>
 </sst>
 </file>
@@ -439,8 +451,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{77884F4D-EAF6-4CE6-A7F9-80362DD9B3E4}" name="Tabla1" displayName="Tabla1" ref="A1:E10" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
-  <autoFilter ref="A1:E10" xr:uid="{77884F4D-EAF6-4CE6-A7F9-80362DD9B3E4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{77884F4D-EAF6-4CE6-A7F9-80362DD9B3E4}" name="Tabla1" displayName="Tabla1" ref="A1:E11" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="A1:E11" xr:uid="{77884F4D-EAF6-4CE6-A7F9-80362DD9B3E4}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{FF02AA83-C173-4DC0-9A0D-43ECBFC0CB7A}" name="Referencia" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{14269345-09BB-4003-8577-05A9C36CF3E7}" name="Nombre" dataDxfId="3"/>
@@ -749,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3001F80C-2A16-4247-B431-82C5DCED0A36}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,6 +935,21 @@
       </c>
       <c r="E10" s="8"/>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="8"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{5F56073C-7AE7-449B-B0C8-6AA479252A6B}"/>

</xml_diff>